<commit_message>
Attendance report filters added
</commit_message>
<xml_diff>
--- a/backend/attendance_tracker/data.xlsx
+++ b/backend/attendance_tracker/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Designations" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -84,21 +84,9 @@
     <t>duration_hours</t>
   </si>
   <si>
-    <t>Test Port 1</t>
-  </si>
-  <si>
-    <t>Test Terminal 1</t>
-  </si>
-  <si>
-    <t>Testing Shift 1</t>
-  </si>
-  <si>
     <t>JNPT_10000135</t>
   </si>
   <si>
-    <t>Test Employee</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -112,6 +100,132 @@
   </si>
   <si>
     <t>Operator</t>
+  </si>
+  <si>
+    <t>JNPA</t>
+  </si>
+  <si>
+    <t>VIZAG</t>
+  </si>
+  <si>
+    <t>Vishakhapattanam</t>
+  </si>
+  <si>
+    <t>KOPT</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>MUNDRA</t>
+  </si>
+  <si>
+    <t>Gujrat</t>
+  </si>
+  <si>
+    <t>HAZIRA</t>
+  </si>
+  <si>
+    <t>MPT</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>South Gate</t>
+  </si>
+  <si>
+    <t>GTI Kiosk</t>
+  </si>
+  <si>
+    <t>Tag Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCTPL Main gate </t>
+  </si>
+  <si>
+    <t>VCTPL Kiosk</t>
+  </si>
+  <si>
+    <t>KOPT KIOSK</t>
+  </si>
+  <si>
+    <t>KOPT ( 8 NO Berth)</t>
+  </si>
+  <si>
+    <t>General shift</t>
+  </si>
+  <si>
+    <t>A shift</t>
+  </si>
+  <si>
+    <t>B shift</t>
+  </si>
+  <si>
+    <t>C shift</t>
+  </si>
+  <si>
+    <t>DAYANAND MHATRE</t>
+  </si>
+  <si>
+    <t>JNPT_10003119</t>
+  </si>
+  <si>
+    <t>NITIN PATIL</t>
+  </si>
+  <si>
+    <t>JNPT_10000171</t>
+  </si>
+  <si>
+    <t>AJIT PATIL</t>
+  </si>
+  <si>
+    <t>JNPT_10000381</t>
+  </si>
+  <si>
+    <t>MANGESH DAS</t>
+  </si>
+  <si>
+    <t>HAZIRA_10001865</t>
+  </si>
+  <si>
+    <t>KALASHI MITESH MANOJBHAI</t>
+  </si>
+  <si>
+    <t>HAZIRA_10001866</t>
+  </si>
+  <si>
+    <t>HAZIRA_10001867</t>
+  </si>
+  <si>
+    <t>HAZIRA_10001868</t>
+  </si>
+  <si>
+    <t>RAMESH SAHU</t>
+  </si>
+  <si>
+    <t>MAHESH SONI</t>
+  </si>
+  <si>
+    <t>RAJESH SHARMA</t>
+  </si>
+  <si>
+    <t>user_type</t>
+  </si>
+  <si>
+    <t>remote_checkin</t>
+  </si>
+  <si>
+    <t>SUPER_ADMIN</t>
+  </si>
+  <si>
+    <t>ADMIN_ADMIN</t>
+  </si>
+  <si>
+    <t>OPERATOR</t>
+  </si>
+  <si>
+    <t>SUPERVISOR</t>
   </si>
 </sst>
 </file>
@@ -167,13 +281,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,39 +571,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Hdfqj7Buy738VhmsazZFuwsp/93bdjcMRavBia1/ZDjaCmKbVP3p5n14m9+t/TmXPEx59s/+NOs1WfkW1T9BqA==" saltValue="cNZMHG9zjqyWrFXa8DKfTA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -494,10 +646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,24 +668,63 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection insertColumns="0" deleteColumns="0" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,18 +754,120 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3">
-        <v>21.829996000000001</v>
+        <v>18.9332821</v>
       </c>
       <c r="D2" s="3">
-        <v>75.630016999999995</v>
+        <v>72.951193900000007</v>
       </c>
       <c r="E2" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3">
+        <v>18.946664699999999</v>
+      </c>
+      <c r="D3" s="3">
+        <v>72.951506699999996</v>
+      </c>
+      <c r="E3" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3">
+        <v>18.9364518</v>
+      </c>
+      <c r="D4" s="3">
+        <v>72.949009500000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3">
+        <v>17.696584999999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>83.299160000000001</v>
+      </c>
+      <c r="E5" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3">
+        <v>17.696321000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <v>83.298832000000004</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3">
+        <v>22.537839999999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>88.302648000000005</v>
+      </c>
+      <c r="E7" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3">
+        <v>22.538872000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>88.300370999999998</v>
+      </c>
+      <c r="E8" s="4">
         <v>100</v>
       </c>
     </row>
@@ -598,16 +891,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
@@ -649,31 +942,234 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2">
-        <v>9999999999</v>
+        <v>45</v>
+      </c>
+      <c r="E2" s="6">
+        <v>8850851141</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
       <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2">
+        <v>31435</v>
+      </c>
+      <c r="J2" s="2">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2">
-        <v>29016</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44951</v>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3">
+        <v>9619461441</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="2">
+        <v>31599</v>
+      </c>
+      <c r="J3" s="2">
+        <v>42992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4">
+        <v>7887465849</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2">
+        <v>32514</v>
+      </c>
+      <c r="J4" s="2">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <v>9619818248</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2">
+        <v>35241</v>
+      </c>
+      <c r="J5" s="2">
+        <v>42584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="6">
+        <v>8850851141</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="2">
+        <v>31435</v>
+      </c>
+      <c r="J6" s="2">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>9619461441</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2">
+        <v>31599</v>
+      </c>
+      <c r="J7" s="2">
+        <v>42992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>7887465849</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2">
+        <v>32514</v>
+      </c>
+      <c r="J8" s="2">
+        <v>42552</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9">
+        <v>9619818248</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2">
+        <v>35241</v>
+      </c>
+      <c r="J9" s="2">
+        <v>42584</v>
       </c>
     </row>
   </sheetData>
@@ -688,15 +1184,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Ports!$A$2:$A$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Designations!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Ports!$A$2:$A$30</xm:f>
-          </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -706,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,10 +1235,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C2" s="5">
         <v>0.375</v>
@@ -752,6 +1248,57 @@
       </c>
       <c r="E2" s="4">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E4" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E5" s="4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>